<commit_message>
Divisão de perfis nos menus.
</commit_message>
<xml_diff>
--- a/dbDumper.xlsx
+++ b/dbDumper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\Dropbox\SESMT\AWS\4\Git Antonio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\Dropbox\SESMT\AWS\4\Git Antonio\GestorSST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7470895A-AC41-4252-BBE1-3EEFD03A61C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3643DDA-F30B-46DA-A273-1E5F6851E5B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20250" yWindow="1815" windowWidth="18150" windowHeight="13035" firstSheet="1" activeTab="5" xr2:uid="{1F2D0AB5-FA2B-4E57-BE55-0836F57ECC8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" activeTab="3" xr2:uid="{1F2D0AB5-FA2B-4E57-BE55-0836F57ECC8F}"/>
   </bookViews>
   <sheets>
     <sheet name="tbEmpresa" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="82">
   <si>
     <t>CNPJ</t>
   </si>
@@ -56,15 +56,6 @@
     <t>UsuarioInclusao</t>
   </si>
   <si>
-    <t>17.155.730/0001-64</t>
-  </si>
-  <si>
-    <t>CIA ENERGETICA DE MINAS GERAIS</t>
-  </si>
-  <si>
-    <t>CEMIG</t>
-  </si>
-  <si>
     <t>superuser</t>
   </si>
   <si>
@@ -110,12 +101,6 @@
     <t>fd1f1c68-9366-4cbd-924e-58f8a41232ae</t>
   </si>
   <si>
-    <t>DPR</t>
-  </si>
-  <si>
-    <t>Presidência</t>
-  </si>
-  <si>
     <t>fba795e7-bc98-4f63-b37b-99b4e21c1e45</t>
   </si>
   <si>
@@ -149,9 +134,6 @@
     <t>711fe4dc-2742-4bc5-beab-238325b23da5</t>
   </si>
   <si>
-    <t>johnnathanalmeida@gmail.com</t>
-  </si>
-  <si>
     <t>UKDepartamento</t>
   </si>
   <si>
@@ -192,13 +174,121 @@
   </si>
   <si>
     <t>URL_WS</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Empregado</t>
+  </si>
+  <si>
+    <t>Técnico</t>
+  </si>
+  <si>
+    <t>Gestor Técnico</t>
+  </si>
+  <si>
+    <t>6d95a771-d6ed-407e-a1e4-12a18dbe17f0</t>
+  </si>
+  <si>
+    <t>6d95a771-d6ed-407e-a1e4-12a18dbe17f1</t>
+  </si>
+  <si>
+    <t>6d95a771-d6ed-407e-a1e4-12a18dbe17f2</t>
+  </si>
+  <si>
+    <t>6d95a771-d6ed-407e-a1e4-12a18dbe17f3</t>
+  </si>
+  <si>
+    <t>6d95a771-d6ed-407e-a1e4-12a18dbe17f4</t>
+  </si>
+  <si>
+    <t>Medicina</t>
+  </si>
+  <si>
+    <t>36.105.882/0001-05</t>
+  </si>
+  <si>
+    <t>MunTec Softwares</t>
+  </si>
+  <si>
+    <t>http://www.muntec.com.br/</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>Tecnologia da Informação</t>
+  </si>
+  <si>
+    <t>959.122.510-55</t>
+  </si>
+  <si>
+    <t>543.803.990-95</t>
+  </si>
+  <si>
+    <t>761.553.710-08</t>
+  </si>
+  <si>
+    <t>957.175.020-44</t>
+  </si>
+  <si>
+    <t>adminuser</t>
+  </si>
+  <si>
+    <t>Admin User</t>
+  </si>
+  <si>
+    <t>Tecnico User</t>
+  </si>
+  <si>
+    <t>Gestor Tecnico User</t>
+  </si>
+  <si>
+    <t>tecnicouser</t>
+  </si>
+  <si>
+    <t>gestortecnicouser</t>
+  </si>
+  <si>
+    <t>245.475.518-12</t>
+  </si>
+  <si>
+    <t>Antônio Henriques</t>
+  </si>
+  <si>
+    <t>antonio</t>
+  </si>
+  <si>
+    <t>Medicina User</t>
+  </si>
+  <si>
+    <t>medicinauser</t>
+  </si>
+  <si>
+    <t>johnnathanalmeida22@gmail.com</t>
+  </si>
+  <si>
+    <t>711fe4dc-2742-4bc5-beab-238325b23da0</t>
+  </si>
+  <si>
+    <t>711fe4dc-2742-4bc5-beab-238325b23da1</t>
+  </si>
+  <si>
+    <t>711fe4dc-2742-4bc5-beab-238325b23da2</t>
+  </si>
+  <si>
+    <t>711fe4dc-2742-4bc5-beab-238325b23da3</t>
+  </si>
+  <si>
+    <t>711fe4dc-2742-4bc5-beab-238325b23da4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +318,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF393939"/>
+      <name val="Open Sans"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -259,6 +354,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -577,21 +673,22 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -609,32 +706,38 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>57</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{12290BE4-1CC1-4282-A797-F4145573A08D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -643,58 +746,58 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -707,72 +810,72 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -782,13 +885,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CA5494-B962-45A6-8753-2D74BC63CC8B}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -798,140 +901,391 @@
     <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6400BF3D-F849-4920-BE1D-9D5FA627F19D}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" customWidth="1"/>
     <col min="7" max="7" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{0C718C56-3D8A-4E69-93C1-B5281F3A2F8B}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{9E1467F5-BB74-42BC-B469-3075881BCCBE}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{A9DD717C-F7D3-4380-99A8-D93653E9A8C8}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{1F84332C-85B1-48E5-8822-7D408AC6D22E}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{249599CC-9E95-40A7-B814-9742FC58E447}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{B52FD2B5-477C-45E7-B845-D3903B4D0A47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -939,13 +1293,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C86F02-B4D4-40D2-A111-D1FC0C648FB3}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
@@ -954,38 +1308,123 @@
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>